<commit_message>
LED Output Driver protocol
LED Output Driver protocol sequence diagram and updated BOM
</commit_message>
<xml_diff>
--- a/Schematic/ECE411_T10_BOM_final.xlsx
+++ b/Schematic/ECE411_T10_BOM_final.xlsx
@@ -593,20 +593,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1308100</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>228592</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>117734</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>138799</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>40602</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Schematic.png"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="schematic.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -625,8 +625,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6629392"/>
-          <a:ext cx="18338001" cy="14896207"/>
+          <a:off x="1917700" y="6350000"/>
+          <a:ext cx="14643100" cy="11877002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>